<commit_message>
update readme, testcases and excel
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunyidan/Library/Mobile Documents/com~apple~CloudDocs/杜克大学/2021spring/ECE568/hw2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunyidan/Downloads/erss-hwk2-ys303-xl350/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A61103-2D2D-1F48-9D5A-3595AFAAA513}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56336F8-9564-734D-A00F-F4108D3AB657}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="1180" windowWidth="29560" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="29560" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Extra note to TA</t>
   </si>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>implement, but has bug</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Please see README</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -106,14 +102,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Every time we get a request from brower, we create a new thread. And we use mutex lock when write to log file and edit cache</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>We lock the cache when we use get and put</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>We lock the logfile when we write to it</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -127,6 +115,18 @@
   </si>
   <si>
     <t>Please find in testcases.txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We cache response that are 200 OK and not private, not no-store</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please see README for details</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Every time we get a request from brower, we create a new thread. And we use mutex lock when writing to log file and editting cache</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -155,6 +155,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -202,6 +203,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -519,7 +521,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="183" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -574,11 +576,11 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" customHeight="1">
@@ -588,6 +590,9 @@
       <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -596,16 +601,19 @@
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="C8" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" customHeight="1">
@@ -623,8 +631,8 @@
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
+      <c r="C11" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="55" customHeight="1">
@@ -634,9 +642,7 @@
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" ht="16" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -646,7 +652,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" customHeight="1">
@@ -665,7 +671,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31" customHeight="1">
@@ -676,7 +682,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1">
@@ -687,7 +693,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1">
@@ -698,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" customHeight="1">

</xml_diff>